<commit_message>
- [x] mapper updates - [x] identifier in listing page - [x] error overwriting fixed - [x] code mapping removed - [x] document link language validation fixed - [x] title language validation fixed - [x] removed code fields from excel mapping - [x] condition country budget item fixed
</commit_message>
<xml_diff>
--- a/public/files/Templates/PeriodXLS.xlsx
+++ b/public/files/Templates/PeriodXLS.xlsx
@@ -4,9 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Instructions" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Period Mapper" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Target Mapper" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Actual Mapper" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Period_Mapper" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Target_Mapper" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Actual_Mapper" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Period" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="Target" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Target Document Link" sheetId="7" r:id="rId10"/>
@@ -30396,7 +30396,7 @@
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Period Mapper'!$C$2:C1000</formula1>
+      <formula1>Period_Mapper!$C$2:C1000</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="E33 C2:C1000">
       <formula1>COUNTIF($C$2:C3,C2)=1</formula1>
@@ -38453,7 +38453,7 @@
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Period Mapper'!$C$2:C1000</formula1>
+      <formula1>Period_Mapper!$C$2:C1000</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that satisfies the formula: =COUNTIF($C$2:C2, C1)&lt;2" sqref="C1:C1000">
       <formula1>COUNTIF($C$2:C2, C1)&lt;2</formula1>
@@ -43537,7 +43537,7 @@
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Period Mapper'!$C$2:$C1000</formula1>
+      <formula1>Period_Mapper!$C$2:$C1000</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -48610,7 +48610,7 @@
       <formula1>Options!$A$2:$A$182</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Target Mapper'!$C$2:C1000</formula1>
+      <formula1>Target_Mapper!$C$2:C1000</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -57695,7 +57695,7 @@
       <formula1>Options!$A$2:$A$182</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Target Mapper'!$C$2:C1000</formula1>
+      <formula1>Target_Mapper!$C$2:C1000</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H1000">
       <formula1>Options!$E$2:$E$31</formula1>
@@ -61772,7 +61772,7 @@
       <formula1>Options!$A$2:$A$182</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Actual Mapper'!$C$2:C1000</formula1>
+      <formula1>Actual_Mapper!$C$2:C1000</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -70856,7 +70856,7 @@
       <formula1>Options!$E$2:$E$31</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>'Actual Mapper'!$C$2:C1000</formula1>
+      <formula1>Actual_Mapper!$C$2:C1000</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>

</xml_diff>